<commit_message>
[docker compose dev] - sucessful for Dockerfile.requirements.dev vs docker-compose.dev (call tới Dockerfile.requirements.dev)    ---- RUN pip install -r requirements.txt -i https://pypi.org/simple  (BỎ NO --CACHE DIR NHANH HẲN, CÒN KHÔNG THÌ 10 MIN)
</commit_message>
<xml_diff>
--- a/queryPostgreSQLDBeaver_log2Larkbase_DIFY/src/backend/api/scripts/query_results/ratings_only.xlsx
+++ b/queryPostgreSQLDBeaver_log2Larkbase_DIFY/src/backend/api/scripts/query_results/ratings_only.xlsx
@@ -335,7 +335,7 @@
 Hãy cùng tìm hiểu nguyên nhân cốt lõi của vấn đề này qua bước dưới đây nhé!</t>
   </si>
   <si>
-    <t>10</t>
+    <t>7</t>
   </si>
   <si>
     <t>2024-11-30 16:16:33</t>
@@ -386,13 +386,13 @@
     <t>2024-12-11 09:41:32</t>
   </si>
   <si>
-    <t>2024-12-12 09:53:43</t>
-  </si>
-  <si>
-    <t>2024-12-12 09:55:30</t>
-  </si>
-  <si>
-    <t>2024-12-12 10:10:33</t>
+    <t>2024-12-12 10:25:26</t>
+  </si>
+  <si>
+    <t>2024-12-12 13:47:28</t>
+  </si>
+  <si>
+    <t>2024-12-12 13:49:33</t>
   </si>
   <si>
     <t>da8ab5b2-b5d0-460d-823b-856592af46ac</t>
@@ -1430,7 +1430,7 @@
         <v>84</v>
       </c>
       <c r="J19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K19" t="s">
         <v>107</v>
@@ -1465,7 +1465,7 @@
         <v>84</v>
       </c>
       <c r="J20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K20" t="s">
         <v>108</v>
@@ -1500,10 +1500,10 @@
         <v>84</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L21" t="s">
         <v>110</v>

</xml_diff>